<commit_message>
Language edits and format responses
Transpose responses so that it is readable. Edit language on pptx.
</commit_message>
<xml_diff>
--- a/BOOK-IT (Responses).xlsx
+++ b/BOOK-IT (Responses).xlsx
@@ -8,14 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rohpl-my.sharepoint.com/personal/admin_rohpl_onmicrosoft_com/Documents/Stephanie/Portfolio/Book-it/bookITrepo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{958656F8-2475-410F-B1D3-B7AD4486B9F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{958656F8-2475-410F-B1D3-B7AD4486B9F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FBE438F-57C4-4B0E-BA48-253FA52F9B03}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="343" windowWidth="22149" windowHeight="12103" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -268,17 +279,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
+    <numFmt numFmtId="168" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -302,11 +308,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,287 +525,323 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:R5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B73B1776-0D94-46CC-BD33-F04FA6FCCA2A}">
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="9" width="21.53515625" customWidth="1"/>
-    <col min="10" max="10" width="34.4609375" customWidth="1"/>
-    <col min="11" max="24" width="21.53515625" customWidth="1"/>
+    <col min="1" max="1" width="99" customWidth="1"/>
+    <col min="2" max="5" width="24.921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="1">
+        <v>44441.084178900463</v>
+      </c>
+      <c r="C1" s="1">
+        <v>44441.086284351855</v>
+      </c>
+      <c r="D1" s="1">
+        <v>44441.575510115741</v>
+      </c>
+      <c r="E1" s="1">
+        <v>44441.862293124999</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>44441.084178900463</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="R2" s="3" t="s">
+      <c r="B18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>44441.086284351855</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="R3" s="3" t="s">
+      <c r="C18" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>44441.575510115741</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="R4" s="3" t="s">
+      <c r="D18" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>44441.862293124999</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>75</v>
+      <c r="E18">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>